<commit_message>
MakeSurvey now getting all survey details. Not updating the database yet.
Changed timetable.xlsx so there are no doube cells
</commit_message>
<xml_diff>
--- a/WiCount/timetable/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/WiCount/timetable/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veldi_000\Dropbox\UCD\Semester3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\veldi_000\git\Assign3\WiCount\timetable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445"/>
   </bookViews>
   <sheets>
     <sheet name="B0.02" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="78">
   <si>
     <t>B0.02</t>
   </si>
@@ -1215,7 +1215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1364,7 +1364,55 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1375,53 +1423,26 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" textRotation="45"/>
@@ -1435,10 +1456,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" textRotation="45"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1462,63 +1519,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1547,16 +1547,69 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1868,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,88 +1952,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="98" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="103"/>
-      <c r="M1" s="100" t="s">
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="101"/>
+      <c r="M1" s="98" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="102" t="s">
+      <c r="O1" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="102"/>
-      <c r="Q1" s="102"/>
-      <c r="R1" s="102"/>
-      <c r="S1" s="102"/>
-      <c r="T1" s="102"/>
-      <c r="U1" s="102"/>
-      <c r="V1" s="102"/>
-      <c r="W1" s="103"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
+      <c r="R1" s="100"/>
+      <c r="S1" s="100"/>
+      <c r="T1" s="100"/>
+      <c r="U1" s="100"/>
+      <c r="V1" s="100"/>
+      <c r="W1" s="101"/>
     </row>
     <row r="2" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="101"/>
+      <c r="A2" s="99"/>
       <c r="B2" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="86" t="s">
+      <c r="D2" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="87"/>
-      <c r="F2" s="86" t="s">
+      <c r="E2" s="103"/>
+      <c r="F2" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="87"/>
-      <c r="H2" s="86" t="s">
+      <c r="G2" s="103"/>
+      <c r="H2" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="88"/>
-      <c r="J2" s="86" t="s">
+      <c r="I2" s="104"/>
+      <c r="J2" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="88"/>
-      <c r="M2" s="101"/>
+      <c r="K2" s="104"/>
+      <c r="M2" s="99"/>
       <c r="N2" s="16" t="s">
         <v>27</v>
       </c>
       <c r="O2" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="86" t="s">
+      <c r="P2" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="87"/>
-      <c r="R2" s="86" t="s">
+      <c r="Q2" s="103"/>
+      <c r="R2" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="87"/>
-      <c r="T2" s="86" t="s">
+      <c r="S2" s="103"/>
+      <c r="T2" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="88"/>
-      <c r="V2" s="86" t="s">
+      <c r="U2" s="104"/>
+      <c r="V2" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="88"/>
+      <c r="W2" s="104"/>
     </row>
     <row r="3" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -2118,10 +2171,10 @@
       <c r="I5" s="13">
         <v>27</v>
       </c>
-      <c r="J5" s="89" t="s">
+      <c r="J5" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="91">
+      <c r="K5" s="168">
         <v>29</v>
       </c>
       <c r="M5" s="15" t="s">
@@ -2147,10 +2200,10 @@
       <c r="U5" s="13">
         <v>27</v>
       </c>
-      <c r="V5" s="89" t="s">
+      <c r="V5" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="W5" s="91">
+      <c r="W5" s="95">
         <v>29</v>
       </c>
     </row>
@@ -2182,8 +2235,12 @@
       <c r="I6" s="14">
         <v>18</v>
       </c>
-      <c r="J6" s="90"/>
-      <c r="K6" s="92"/>
+      <c r="J6" s="165" t="s">
+        <v>2</v>
+      </c>
+      <c r="K6" s="168">
+        <v>29</v>
+      </c>
       <c r="M6" s="15" t="s">
         <v>21</v>
       </c>
@@ -2211,8 +2268,8 @@
       <c r="U6" s="14">
         <v>18</v>
       </c>
-      <c r="V6" s="90"/>
-      <c r="W6" s="92"/>
+      <c r="V6" s="88"/>
+      <c r="W6" s="96"/>
     </row>
     <row r="7" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -2284,10 +2341,10 @@
       <c r="C8" s="10">
         <v>18</v>
       </c>
-      <c r="D8" s="89" t="s">
+      <c r="D8" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="97">
+      <c r="E8" s="167">
         <v>42</v>
       </c>
       <c r="F8" s="22" t="s">
@@ -2317,7 +2374,7 @@
       <c r="O8" s="10">
         <v>18</v>
       </c>
-      <c r="P8" s="89" t="s">
+      <c r="P8" s="87" t="s">
         <v>7</v>
       </c>
       <c r="Q8" s="97">
@@ -2348,18 +2405,22 @@
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="96"/>
+      <c r="D9" s="165" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="167">
+        <v>42</v>
+      </c>
       <c r="F9" s="24" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="4">
         <v>79</v>
       </c>
-      <c r="H9" s="93" t="s">
+      <c r="H9" s="166" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="91">
+      <c r="I9" s="168">
         <v>60</v>
       </c>
       <c r="J9" s="34"/>
@@ -2369,18 +2430,18 @@
       </c>
       <c r="N9" s="20"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="90"/>
-      <c r="Q9" s="96"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="94"/>
       <c r="R9" s="24" t="s">
         <v>17</v>
       </c>
       <c r="S9" s="4">
         <v>79</v>
       </c>
-      <c r="T9" s="93" t="s">
+      <c r="T9" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="U9" s="91">
+      <c r="U9" s="95">
         <v>60</v>
       </c>
       <c r="V9" s="34"/>
@@ -2390,51 +2451,55 @@
       <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="89" t="s">
+      <c r="B10" s="165" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="98">
+      <c r="C10" s="163">
         <v>53</v>
       </c>
-      <c r="D10" s="93" t="s">
+      <c r="D10" s="166" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="95">
+      <c r="E10" s="164">
         <v>27</v>
       </c>
-      <c r="F10" s="93" t="s">
+      <c r="F10" s="166" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="95">
+      <c r="G10" s="93">
         <v>22</v>
       </c>
-      <c r="H10" s="94"/>
-      <c r="I10" s="92"/>
+      <c r="H10" s="166" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="168">
+        <v>60</v>
+      </c>
       <c r="J10" s="34"/>
       <c r="K10" s="31"/>
       <c r="M10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="89" t="s">
+      <c r="N10" s="87" t="s">
         <v>12</v>
       </c>
-      <c r="O10" s="98">
+      <c r="O10" s="89">
         <v>53</v>
       </c>
-      <c r="P10" s="93" t="s">
+      <c r="P10" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="Q10" s="95">
+      <c r="Q10" s="93">
         <v>27</v>
       </c>
-      <c r="R10" s="93" t="s">
+      <c r="R10" s="91" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="95">
+      <c r="S10" s="93">
         <v>22</v>
       </c>
-      <c r="T10" s="94"/>
-      <c r="U10" s="92"/>
+      <c r="T10" s="92"/>
+      <c r="U10" s="96"/>
       <c r="V10" s="34"/>
       <c r="W10" s="31"/>
     </row>
@@ -2442,12 +2507,22 @@
       <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="96"/>
+      <c r="B11" s="165" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="163">
+        <v>53</v>
+      </c>
+      <c r="D11" s="166" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="164">
+        <v>27</v>
+      </c>
+      <c r="F11" s="166" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="94"/>
       <c r="H11" s="21"/>
       <c r="I11" s="25"/>
       <c r="J11" s="20"/>
@@ -2456,12 +2531,12 @@
       <c r="M11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="90"/>
-      <c r="O11" s="99"/>
-      <c r="P11" s="94"/>
-      <c r="Q11" s="96"/>
-      <c r="R11" s="94"/>
-      <c r="S11" s="96"/>
+      <c r="N11" s="88"/>
+      <c r="O11" s="90"/>
+      <c r="P11" s="92"/>
+      <c r="Q11" s="94"/>
+      <c r="R11" s="92"/>
+      <c r="S11" s="94"/>
       <c r="T11" s="21"/>
       <c r="U11" s="25"/>
       <c r="V11" s="20"/>
@@ -2480,75 +2555,45 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="N13" s="104"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
-      <c r="U13" s="104"/>
-      <c r="V13" s="104"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="85"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="85"/>
+      <c r="U13" s="85"/>
+      <c r="V13" s="85"/>
     </row>
     <row r="14" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="60" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="86"/>
+      <c r="S14" s="86"/>
+      <c r="T14" s="86"/>
+      <c r="U14" s="86"/>
+      <c r="V14" s="86"/>
+      <c r="W14" s="86"/>
     </row>
     <row r="15" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="N13:V13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="O1:W1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="E8:E9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:K1"/>
+  <mergeCells count="35">
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
@@ -2557,14 +2602,33 @@
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="F10:F11"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="O1:W1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="W5:W6"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="Q8:Q9"/>
+    <mergeCell ref="T9:T10"/>
+    <mergeCell ref="U9:U10"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="Q10:Q11"/>
+    <mergeCell ref="R10:R11"/>
+    <mergeCell ref="N13:V13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2576,8 +2640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2607,97 +2671,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111" t="s">
+      <c r="A1" s="130" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="113"/>
-      <c r="G1" s="113"/>
-      <c r="H1" s="113"/>
-      <c r="I1" s="113"/>
-      <c r="J1" s="113"/>
-      <c r="K1" s="114"/>
-      <c r="M1" s="111" t="s">
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="132"/>
+      <c r="G1" s="132"/>
+      <c r="H1" s="132"/>
+      <c r="I1" s="132"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="133"/>
+      <c r="M1" s="130" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="113" t="s">
+      <c r="O1" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="113"/>
-      <c r="Q1" s="113"/>
-      <c r="R1" s="113"/>
-      <c r="S1" s="113"/>
-      <c r="T1" s="113"/>
-      <c r="U1" s="113"/>
-      <c r="V1" s="113"/>
-      <c r="W1" s="114"/>
+      <c r="P1" s="132"/>
+      <c r="Q1" s="132"/>
+      <c r="R1" s="132"/>
+      <c r="S1" s="132"/>
+      <c r="T1" s="132"/>
+      <c r="U1" s="132"/>
+      <c r="V1" s="132"/>
+      <c r="W1" s="133"/>
     </row>
     <row r="2" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="112"/>
+      <c r="A2" s="131"/>
       <c r="B2" s="38" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="115" t="s">
+      <c r="D2" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="116"/>
-      <c r="F2" s="115" t="s">
+      <c r="E2" s="135"/>
+      <c r="F2" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="116"/>
-      <c r="H2" s="115" t="s">
+      <c r="G2" s="135"/>
+      <c r="H2" s="134" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="117"/>
-      <c r="J2" s="115" t="s">
+      <c r="I2" s="136"/>
+      <c r="J2" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="117"/>
-      <c r="M2" s="112"/>
+      <c r="K2" s="136"/>
+      <c r="M2" s="131"/>
       <c r="N2" s="38" t="s">
         <v>27</v>
       </c>
       <c r="O2" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="P2" s="115" t="s">
+      <c r="P2" s="134" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="116"/>
-      <c r="R2" s="115" t="s">
+      <c r="Q2" s="135"/>
+      <c r="R2" s="134" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="116"/>
-      <c r="T2" s="115" t="s">
+      <c r="S2" s="135"/>
+      <c r="T2" s="134" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="117"/>
-      <c r="V2" s="115" t="s">
+      <c r="U2" s="136"/>
+      <c r="V2" s="134" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="117"/>
+      <c r="W2" s="136"/>
     </row>
     <row r="3" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="107">
+      <c r="C3" s="148">
         <v>53</v>
       </c>
       <c r="D3" s="54"/>
@@ -2714,19 +2778,19 @@
       <c r="I3" s="42">
         <v>42</v>
       </c>
-      <c r="J3" s="105" t="s">
+      <c r="J3" s="149" t="s">
         <v>35</v>
       </c>
-      <c r="K3" s="109">
+      <c r="K3" s="156">
         <v>45</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="105" t="s">
+      <c r="N3" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="O3" s="107">
+      <c r="O3" s="114">
         <v>53</v>
       </c>
       <c r="P3" s="54"/>
@@ -2743,10 +2807,10 @@
       <c r="U3" s="42">
         <v>42</v>
       </c>
-      <c r="V3" s="105" t="s">
+      <c r="V3" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="W3" s="109">
+      <c r="W3" s="107">
         <v>45</v>
       </c>
     </row>
@@ -2754,46 +2818,54 @@
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="108"/>
+      <c r="B4" s="149" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="148">
+        <v>53</v>
+      </c>
       <c r="D4" s="46"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="131" t="s">
+      <c r="F4" s="153" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="129">
+      <c r="G4" s="151">
         <v>0</v>
       </c>
       <c r="H4" s="54"/>
       <c r="I4" s="55"/>
-      <c r="J4" s="106"/>
-      <c r="K4" s="110"/>
+      <c r="J4" s="149" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" s="156">
+        <v>45</v>
+      </c>
       <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="106"/>
-      <c r="O4" s="108"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="115"/>
       <c r="P4" s="46"/>
       <c r="Q4" s="6"/>
-      <c r="R4" s="131" t="s">
+      <c r="R4" s="108" t="s">
         <v>43</v>
       </c>
-      <c r="S4" s="129">
+      <c r="S4" s="110">
         <v>0</v>
       </c>
       <c r="T4" s="54"/>
       <c r="U4" s="55"/>
-      <c r="V4" s="106"/>
-      <c r="W4" s="110"/>
+      <c r="V4" s="113"/>
+      <c r="W4" s="106"/>
     </row>
     <row r="5" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="105" t="s">
+      <c r="B5" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="107">
+      <c r="C5" s="148">
         <v>45</v>
       </c>
       <c r="D5" s="40" t="s">
@@ -2802,23 +2874,27 @@
       <c r="E5" s="41">
         <v>56</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="130"/>
+      <c r="F5" s="153" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="151">
+        <v>0</v>
+      </c>
       <c r="H5" s="46"/>
       <c r="I5" s="56"/>
-      <c r="J5" s="118" t="s">
+      <c r="J5" s="159" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="120">
+      <c r="K5" s="157">
         <v>0</v>
       </c>
       <c r="M5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="105" t="s">
+      <c r="N5" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="O5" s="107">
+      <c r="O5" s="114">
         <v>45</v>
       </c>
       <c r="P5" s="40" t="s">
@@ -2827,11 +2903,11 @@
       <c r="Q5" s="41">
         <v>56</v>
       </c>
-      <c r="R5" s="132"/>
-      <c r="S5" s="130"/>
+      <c r="R5" s="109"/>
+      <c r="S5" s="111"/>
       <c r="T5" s="46"/>
       <c r="U5" s="56"/>
-      <c r="V5" s="118" t="s">
+      <c r="V5" s="127" t="s">
         <v>10</v>
       </c>
       <c r="W5" s="120">
@@ -2842,14 +2918,18 @@
       <c r="A6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="106"/>
-      <c r="C6" s="108"/>
+      <c r="B6" s="149" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="148">
+        <v>45</v>
+      </c>
       <c r="D6" s="46"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="135" t="s">
+      <c r="F6" s="154" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="127">
+      <c r="G6" s="152">
         <v>73</v>
       </c>
       <c r="H6" s="43" t="s">
@@ -2858,19 +2938,23 @@
       <c r="I6" s="44">
         <v>56</v>
       </c>
-      <c r="J6" s="119"/>
-      <c r="K6" s="121"/>
+      <c r="J6" s="159" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="157">
+        <v>0</v>
+      </c>
       <c r="M6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="106"/>
-      <c r="O6" s="108"/>
+      <c r="N6" s="113"/>
+      <c r="O6" s="115"/>
       <c r="P6" s="46"/>
       <c r="Q6" s="6"/>
-      <c r="R6" s="135" t="s">
+      <c r="R6" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="S6" s="127">
+      <c r="S6" s="118">
         <v>73</v>
       </c>
       <c r="T6" s="43" t="s">
@@ -2879,7 +2963,7 @@
       <c r="U6" s="44">
         <v>56</v>
       </c>
-      <c r="V6" s="119"/>
+      <c r="V6" s="128"/>
       <c r="W6" s="121"/>
     </row>
     <row r="7" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2894,16 +2978,20 @@
       <c r="E7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="136"/>
-      <c r="G7" s="128"/>
+      <c r="F7" s="154" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="152">
+        <v>73</v>
+      </c>
       <c r="H7" s="45" t="s">
         <v>39</v>
       </c>
       <c r="I7" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="26"/>
+      <c r="J7" s="160"/>
+      <c r="K7" s="161"/>
       <c r="M7" s="15" t="s">
         <v>22</v>
       </c>
@@ -2915,8 +3003,8 @@
       <c r="Q7" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="R7" s="136"/>
-      <c r="S7" s="128"/>
+      <c r="R7" s="117"/>
+      <c r="S7" s="119"/>
       <c r="T7" s="45" t="s">
         <v>39</v>
       </c>
@@ -2930,18 +3018,18 @@
       <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="105" t="s">
+      <c r="B8" s="149" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="133">
+      <c r="C8" s="150">
         <v>33</v>
       </c>
       <c r="D8" s="47"/>
       <c r="E8" s="48"/>
-      <c r="F8" s="122" t="s">
+      <c r="F8" s="155" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="129">
+      <c r="G8" s="151">
         <v>0</v>
       </c>
       <c r="H8" s="29" t="s">
@@ -2950,27 +3038,27 @@
       <c r="I8" s="62">
         <v>0</v>
       </c>
-      <c r="J8" s="105" t="s">
+      <c r="J8" s="149" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="126">
+      <c r="K8" s="158">
         <v>65</v>
       </c>
       <c r="M8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="105" t="s">
+      <c r="N8" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="O8" s="133">
+      <c r="O8" s="122">
         <v>33</v>
       </c>
       <c r="P8" s="47"/>
       <c r="Q8" s="48"/>
-      <c r="R8" s="122" t="s">
+      <c r="R8" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="S8" s="129">
+      <c r="S8" s="110">
         <v>0</v>
       </c>
       <c r="T8" s="29" t="s">
@@ -2979,10 +3067,10 @@
       <c r="U8" s="62">
         <v>0</v>
       </c>
-      <c r="V8" s="105" t="s">
+      <c r="V8" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="W8" s="126">
+      <c r="W8" s="105">
         <v>65</v>
       </c>
     </row>
@@ -2990,56 +3078,68 @@
       <c r="A9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="106"/>
-      <c r="C9" s="134"/>
+      <c r="B9" s="149" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="150">
+        <v>33</v>
+      </c>
       <c r="D9" s="49"/>
       <c r="E9" s="50"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="130"/>
+      <c r="F9" s="155" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="151">
+        <v>0</v>
+      </c>
       <c r="H9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="62">
         <v>0</v>
       </c>
-      <c r="J9" s="125"/>
-      <c r="K9" s="110"/>
+      <c r="J9" s="149" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9" s="158">
+        <v>65</v>
+      </c>
       <c r="M9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="106"/>
-      <c r="O9" s="134"/>
+      <c r="N9" s="113"/>
+      <c r="O9" s="123"/>
       <c r="P9" s="49"/>
       <c r="Q9" s="50"/>
-      <c r="R9" s="123"/>
-      <c r="S9" s="130"/>
+      <c r="R9" s="125"/>
+      <c r="S9" s="111"/>
       <c r="T9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="U9" s="62">
         <v>0</v>
       </c>
-      <c r="V9" s="125"/>
-      <c r="W9" s="110"/>
+      <c r="V9" s="126"/>
+      <c r="W9" s="106"/>
     </row>
     <row r="10" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="105" t="s">
+      <c r="B10" s="149" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="107">
+      <c r="C10" s="148">
         <v>35</v>
       </c>
       <c r="D10" s="51"/>
       <c r="E10" s="52"/>
       <c r="F10" s="51"/>
       <c r="G10" s="52"/>
-      <c r="H10" s="122" t="s">
+      <c r="H10" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="124">
+      <c r="I10" s="162">
         <v>0</v>
       </c>
       <c r="J10" s="34"/>
@@ -3047,20 +3147,20 @@
       <c r="M10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="105" t="s">
+      <c r="N10" s="112" t="s">
         <v>37</v>
       </c>
-      <c r="O10" s="107">
+      <c r="O10" s="114">
         <v>35</v>
       </c>
       <c r="P10" s="51"/>
       <c r="Q10" s="52"/>
       <c r="R10" s="51"/>
       <c r="S10" s="52"/>
-      <c r="T10" s="122" t="s">
+      <c r="T10" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="U10" s="124">
+      <c r="U10" s="129">
         <v>0</v>
       </c>
       <c r="V10" s="34"/>
@@ -3070,27 +3170,35 @@
       <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="106"/>
-      <c r="C11" s="108"/>
+      <c r="B11" s="149" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="148">
+        <v>35</v>
+      </c>
       <c r="D11" s="53"/>
       <c r="E11" s="50"/>
       <c r="F11" s="53"/>
       <c r="G11" s="50"/>
-      <c r="H11" s="123"/>
-      <c r="I11" s="121"/>
+      <c r="H11" s="155" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="162">
+        <v>0</v>
+      </c>
       <c r="J11" s="20"/>
       <c r="K11" s="32"/>
       <c r="L11" s="35"/>
       <c r="M11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="106"/>
-      <c r="O11" s="108"/>
+      <c r="N11" s="113"/>
+      <c r="O11" s="115"/>
       <c r="P11" s="53"/>
       <c r="Q11" s="50"/>
       <c r="R11" s="53"/>
       <c r="S11" s="50"/>
-      <c r="T11" s="123"/>
+      <c r="T11" s="125"/>
       <c r="U11" s="121"/>
       <c r="V11" s="20"/>
       <c r="W11" s="32"/>
@@ -3108,45 +3216,75 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="N13" s="104"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
-      <c r="U13" s="104"/>
-      <c r="V13" s="104"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="85"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="85"/>
+      <c r="U13" s="85"/>
+      <c r="V13" s="85"/>
     </row>
     <row r="14" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="60" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="86"/>
+      <c r="S14" s="86"/>
+      <c r="T14" s="86"/>
+      <c r="U14" s="86"/>
+      <c r="V14" s="86"/>
+      <c r="W14" s="86"/>
     </row>
     <row r="15" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="44">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="O1:W1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="V5:V6"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="N13:V13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
     <mergeCell ref="W8:W9"/>
     <mergeCell ref="W3:W4"/>
     <mergeCell ref="R4:R5"/>
@@ -3161,58 +3299,6 @@
     <mergeCell ref="R8:R9"/>
     <mergeCell ref="S8:S9"/>
     <mergeCell ref="V8:V9"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="N13:V13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="O1:W1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3223,8 +3309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3404,7 +3490,7 @@
       <c r="B4" s="146" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="148">
+      <c r="C4" s="147">
         <v>49</v>
       </c>
       <c r="D4" s="65" t="s">
@@ -3457,8 +3543,12 @@
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="147"/>
-      <c r="C5" s="149"/>
+      <c r="B5" s="146" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="147">
+        <v>49</v>
+      </c>
       <c r="D5" s="65" t="s">
         <v>53</v>
       </c>
@@ -3827,57 +3917,45 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="N13" s="104"/>
-      <c r="O13" s="104"/>
-      <c r="P13" s="104"/>
-      <c r="Q13" s="104"/>
-      <c r="R13" s="104"/>
-      <c r="S13" s="104"/>
-      <c r="T13" s="104"/>
-      <c r="U13" s="104"/>
-      <c r="V13" s="104"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="85"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="85"/>
+      <c r="U13" s="85"/>
+      <c r="V13" s="85"/>
     </row>
     <row r="14" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="60" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="85"/>
-      <c r="F14" s="85"/>
-      <c r="G14" s="85"/>
-      <c r="H14" s="85"/>
-      <c r="I14" s="85"/>
-      <c r="J14" s="85"/>
-      <c r="K14" s="85"/>
-      <c r="N14" s="85"/>
-      <c r="O14" s="85"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="85"/>
-      <c r="R14" s="85"/>
-      <c r="S14" s="85"/>
-      <c r="T14" s="85"/>
-      <c r="U14" s="85"/>
-      <c r="V14" s="85"/>
-      <c r="W14" s="85"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="N14" s="86"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
+      <c r="R14" s="86"/>
+      <c r="S14" s="86"/>
+      <c r="T14" s="86"/>
+      <c r="U14" s="86"/>
+      <c r="V14" s="86"/>
+      <c r="W14" s="86"/>
     </row>
     <row r="15" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="24">
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="N13:V13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
+  <mergeCells count="22">
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="A1:A2"/>
@@ -3890,6 +3968,16 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="N13:V13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Added week Number field to the timetable table.
</commit_message>
<xml_diff>
--- a/WiCount/timetable/B0.02 B0.03 B0.04 Timetable.xlsx
+++ b/WiCount/timetable/B0.02 B0.03 B0.04 Timetable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="B0.02" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="79">
   <si>
     <t>B0.02</t>
   </si>
@@ -465,12 +465,6 @@
     <t>Friday 6th</t>
   </si>
   <si>
-    <t>2 Nov - 6 Nov</t>
-  </si>
-  <si>
-    <t>9 Nov - 13 Nov</t>
-  </si>
-  <si>
     <t xml:space="preserve">No. of registered students </t>
   </si>
   <si>
@@ -601,6 +595,15 @@
   </si>
   <si>
     <t>Room capacity: 90</t>
+  </si>
+  <si>
+    <t>9 Nov 2015 - 13 Nov 2015</t>
+  </si>
+  <si>
+    <t>2 Nov 2015 - 6 Nov 2015</t>
+  </si>
+  <si>
+    <t>9 Nov 2015- 13 Nov 2015</t>
   </si>
 </sst>
 </file>
@@ -696,7 +699,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="39">
     <border>
       <left/>
       <right/>
@@ -1021,7 +1024,20 @@
         <color theme="2" tint="-0.749992370372631"/>
       </left>
       <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
       </right>
       <top/>
       <bottom style="thin">
@@ -1036,32 +1052,6 @@
       <right style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1073,36 +1063,10 @@
       <right style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dotted">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
       <top style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="dotted">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1215,7 +1179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="135">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1300,7 +1264,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1319,19 +1283,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="45"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" textRotation="45"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1354,150 +1318,113 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" textRotation="45"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1540,76 +1467,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1921,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:K6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,88 +1814,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="98" t="s">
+      <c r="A1" s="114" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="100" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="101"/>
-      <c r="M1" s="98" t="s">
+      <c r="C1" s="116" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="116"/>
+      <c r="E1" s="116"/>
+      <c r="F1" s="116"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="117"/>
+      <c r="M1" s="114" t="s">
         <v>0</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="100" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="100"/>
-      <c r="Q1" s="100"/>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="101"/>
+        <v>76</v>
+      </c>
+      <c r="O1" s="116" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="116"/>
+      <c r="Q1" s="116"/>
+      <c r="R1" s="116"/>
+      <c r="S1" s="116"/>
+      <c r="T1" s="116"/>
+      <c r="U1" s="116"/>
+      <c r="V1" s="116"/>
+      <c r="W1" s="117"/>
     </row>
     <row r="2" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="99"/>
+      <c r="A2" s="115"/>
       <c r="B2" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="103"/>
-      <c r="F2" s="102" t="s">
+      <c r="E2" s="110"/>
+      <c r="F2" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="103"/>
-      <c r="H2" s="102" t="s">
+      <c r="G2" s="110"/>
+      <c r="H2" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="104"/>
-      <c r="J2" s="102" t="s">
+      <c r="I2" s="111"/>
+      <c r="J2" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="104"/>
-      <c r="M2" s="99"/>
+      <c r="K2" s="111"/>
+      <c r="M2" s="115"/>
       <c r="N2" s="16" t="s">
         <v>27</v>
       </c>
       <c r="O2" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="102" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="103"/>
-      <c r="R2" s="102" t="s">
+      <c r="Q2" s="110"/>
+      <c r="R2" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="103"/>
-      <c r="T2" s="102" t="s">
+      <c r="S2" s="110"/>
+      <c r="T2" s="109" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="104"/>
-      <c r="V2" s="102" t="s">
+      <c r="U2" s="111"/>
+      <c r="V2" s="109" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="104"/>
+      <c r="W2" s="111"/>
     </row>
     <row r="3" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
@@ -2171,10 +2033,10 @@
       <c r="I5" s="13">
         <v>27</v>
       </c>
-      <c r="J5" s="165" t="s">
+      <c r="J5" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="K5" s="168">
+      <c r="K5" s="107">
         <v>29</v>
       </c>
       <c r="M5" s="15" t="s">
@@ -2200,10 +2062,10 @@
       <c r="U5" s="13">
         <v>27</v>
       </c>
-      <c r="V5" s="87" t="s">
+      <c r="V5" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="W5" s="95">
+      <c r="W5" s="107">
         <v>29</v>
       </c>
     </row>
@@ -2235,10 +2097,10 @@
       <c r="I6" s="14">
         <v>18</v>
       </c>
-      <c r="J6" s="165" t="s">
+      <c r="J6" s="104" t="s">
         <v>2</v>
       </c>
-      <c r="K6" s="168">
+      <c r="K6" s="107">
         <v>29</v>
       </c>
       <c r="M6" s="15" t="s">
@@ -2268,8 +2130,12 @@
       <c r="U6" s="14">
         <v>18</v>
       </c>
-      <c r="V6" s="88"/>
-      <c r="W6" s="96"/>
+      <c r="V6" s="104" t="s">
+        <v>2</v>
+      </c>
+      <c r="W6" s="107">
+        <v>29</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -2341,10 +2207,10 @@
       <c r="C8" s="10">
         <v>18</v>
       </c>
-      <c r="D8" s="165" t="s">
+      <c r="D8" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="167">
+      <c r="E8" s="106">
         <v>42</v>
       </c>
       <c r="F8" s="22" t="s">
@@ -2374,10 +2240,10 @@
       <c r="O8" s="10">
         <v>18</v>
       </c>
-      <c r="P8" s="87" t="s">
+      <c r="P8" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="Q8" s="97">
+      <c r="Q8" s="106">
         <v>42</v>
       </c>
       <c r="R8" s="22" t="s">
@@ -2405,10 +2271,10 @@
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="11"/>
-      <c r="D9" s="165" t="s">
+      <c r="D9" s="104" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="167">
+      <c r="E9" s="106">
         <v>42</v>
       </c>
       <c r="F9" s="24" t="s">
@@ -2417,10 +2283,10 @@
       <c r="G9" s="4">
         <v>79</v>
       </c>
-      <c r="H9" s="166" t="s">
+      <c r="H9" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="168">
+      <c r="I9" s="107">
         <v>60</v>
       </c>
       <c r="J9" s="34"/>
@@ -2430,18 +2296,22 @@
       </c>
       <c r="N9" s="20"/>
       <c r="O9" s="11"/>
-      <c r="P9" s="88"/>
-      <c r="Q9" s="94"/>
+      <c r="P9" s="104" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q9" s="106">
+        <v>42</v>
+      </c>
       <c r="R9" s="24" t="s">
         <v>17</v>
       </c>
       <c r="S9" s="4">
         <v>79</v>
       </c>
-      <c r="T9" s="91" t="s">
+      <c r="T9" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="U9" s="95">
+      <c r="U9" s="107">
         <v>60</v>
       </c>
       <c r="V9" s="34"/>
@@ -2451,28 +2321,28 @@
       <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="165" t="s">
+      <c r="B10" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="163">
+      <c r="C10" s="102">
         <v>53</v>
       </c>
-      <c r="D10" s="166" t="s">
+      <c r="D10" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="164">
+      <c r="E10" s="103">
         <v>27</v>
       </c>
-      <c r="F10" s="166" t="s">
+      <c r="F10" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="93">
+      <c r="G10" s="112">
         <v>22</v>
       </c>
-      <c r="H10" s="166" t="s">
+      <c r="H10" s="105" t="s">
         <v>11</v>
       </c>
-      <c r="I10" s="168">
+      <c r="I10" s="107">
         <v>60</v>
       </c>
       <c r="J10" s="34"/>
@@ -2480,26 +2350,30 @@
       <c r="M10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="87" t="s">
+      <c r="N10" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="O10" s="89">
+      <c r="O10" s="102">
         <v>53</v>
       </c>
-      <c r="P10" s="91" t="s">
+      <c r="P10" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="Q10" s="93">
+      <c r="Q10" s="103">
         <v>27</v>
       </c>
-      <c r="R10" s="91" t="s">
+      <c r="R10" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="S10" s="93">
+      <c r="S10" s="112">
         <v>22</v>
       </c>
-      <c r="T10" s="92"/>
-      <c r="U10" s="96"/>
+      <c r="T10" s="105" t="s">
+        <v>11</v>
+      </c>
+      <c r="U10" s="107">
+        <v>60</v>
+      </c>
       <c r="V10" s="34"/>
       <c r="W10" s="31"/>
     </row>
@@ -2507,22 +2381,22 @@
       <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="165" t="s">
+      <c r="B11" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="163">
+      <c r="C11" s="102">
         <v>53</v>
       </c>
-      <c r="D11" s="166" t="s">
+      <c r="D11" s="105" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="164">
+      <c r="E11" s="103">
         <v>27</v>
       </c>
-      <c r="F11" s="166" t="s">
+      <c r="F11" s="105" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="94"/>
+      <c r="G11" s="113"/>
       <c r="H11" s="21"/>
       <c r="I11" s="25"/>
       <c r="J11" s="20"/>
@@ -2531,12 +2405,22 @@
       <c r="M11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="88"/>
-      <c r="O11" s="90"/>
-      <c r="P11" s="92"/>
-      <c r="Q11" s="94"/>
-      <c r="R11" s="92"/>
-      <c r="S11" s="94"/>
+      <c r="N11" s="104" t="s">
+        <v>12</v>
+      </c>
+      <c r="O11" s="102">
+        <v>53</v>
+      </c>
+      <c r="P11" s="105" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q11" s="103">
+        <v>27</v>
+      </c>
+      <c r="R11" s="105" t="s">
+        <v>13</v>
+      </c>
+      <c r="S11" s="113"/>
       <c r="T11" s="21"/>
       <c r="U11" s="25"/>
       <c r="V11" s="20"/>
@@ -2545,7 +2429,7 @@
     <row r="12" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="59" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2555,45 +2439,60 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85"/>
-      <c r="R13" s="85"/>
-      <c r="S13" s="85"/>
-      <c r="T13" s="85"/>
-      <c r="U13" s="85"/>
-      <c r="V13" s="85"/>
+      <c r="N13" s="118"/>
+      <c r="O13" s="118"/>
+      <c r="P13" s="118"/>
+      <c r="Q13" s="118"/>
+      <c r="R13" s="118"/>
+      <c r="S13" s="118"/>
+      <c r="T13" s="118"/>
+      <c r="U13" s="118"/>
+      <c r="V13" s="118"/>
     </row>
     <row r="14" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="86"/>
-      <c r="Q14" s="86"/>
-      <c r="R14" s="86"/>
-      <c r="S14" s="86"/>
-      <c r="T14" s="86"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="86"/>
-      <c r="W14" s="86"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="108"/>
+      <c r="K14" s="108"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
+      <c r="U14" s="108"/>
+      <c r="V14" s="108"/>
+      <c r="W14" s="108"/>
     </row>
     <row r="15" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="35">
+  <mergeCells count="24">
+    <mergeCell ref="N13:V13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="S10:S11"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:K1"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="O1:W1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="H14:I14"/>
@@ -2603,32 +2502,6 @@
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="G10:G11"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:K1"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="O1:W1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="S10:S11"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="Q8:Q9"/>
-    <mergeCell ref="T9:T10"/>
-    <mergeCell ref="U9:U10"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="Q10:Q11"/>
-    <mergeCell ref="R10:R11"/>
-    <mergeCell ref="N13:V13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2640,8 +2513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:I11"/>
+    <sheetView topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5:W6 R6:S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2671,146 +2544,146 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="119" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="132"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="132"/>
-      <c r="G1" s="132"/>
-      <c r="H1" s="132"/>
-      <c r="I1" s="132"/>
-      <c r="J1" s="132"/>
-      <c r="K1" s="133"/>
-      <c r="M1" s="130" t="s">
+      <c r="C1" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="122"/>
+      <c r="M1" s="119" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="132" t="s">
-        <v>77</v>
-      </c>
-      <c r="P1" s="132"/>
-      <c r="Q1" s="132"/>
-      <c r="R1" s="132"/>
-      <c r="S1" s="132"/>
-      <c r="T1" s="132"/>
-      <c r="U1" s="132"/>
-      <c r="V1" s="132"/>
-      <c r="W1" s="133"/>
+        <v>76</v>
+      </c>
+      <c r="O1" s="121" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="121"/>
+      <c r="R1" s="121"/>
+      <c r="S1" s="121"/>
+      <c r="T1" s="121"/>
+      <c r="U1" s="121"/>
+      <c r="V1" s="121"/>
+      <c r="W1" s="122"/>
     </row>
     <row r="2" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="131"/>
+      <c r="A2" s="120"/>
       <c r="B2" s="38" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="134" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="135"/>
-      <c r="F2" s="134" t="s">
+      <c r="E2" s="124"/>
+      <c r="F2" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="135"/>
-      <c r="H2" s="134" t="s">
+      <c r="G2" s="124"/>
+      <c r="H2" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="136"/>
-      <c r="J2" s="134" t="s">
+      <c r="I2" s="125"/>
+      <c r="J2" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="136"/>
-      <c r="M2" s="131"/>
+      <c r="K2" s="125"/>
+      <c r="M2" s="120"/>
       <c r="N2" s="38" t="s">
         <v>27</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="134" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="123" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="135"/>
-      <c r="R2" s="134" t="s">
+      <c r="Q2" s="124"/>
+      <c r="R2" s="123" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="135"/>
-      <c r="T2" s="134" t="s">
+      <c r="S2" s="124"/>
+      <c r="T2" s="123" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="136"/>
-      <c r="V2" s="134" t="s">
+      <c r="U2" s="125"/>
+      <c r="V2" s="123" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="136"/>
+      <c r="W2" s="125"/>
     </row>
     <row r="3" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="149" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="148">
+      <c r="B3" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="87">
         <v>53</v>
       </c>
       <c r="D3" s="54"/>
       <c r="E3" s="57"/>
       <c r="F3" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
       </c>
       <c r="H3" s="40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I3" s="42">
         <v>42</v>
       </c>
-      <c r="J3" s="149" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="156">
+      <c r="J3" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="95">
         <v>45</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="112" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="114">
+      <c r="N3" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="87">
         <v>53</v>
       </c>
       <c r="P3" s="54"/>
       <c r="Q3" s="57"/>
       <c r="R3" s="29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S3" s="5">
         <v>0</v>
       </c>
       <c r="T3" s="40" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="U3" s="42">
         <v>42</v>
       </c>
-      <c r="V3" s="112" t="s">
-        <v>35</v>
-      </c>
-      <c r="W3" s="107">
+      <c r="V3" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="W3" s="95">
         <v>45</v>
       </c>
     </row>
@@ -2818,99 +2691,111 @@
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="149" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="148">
+      <c r="B4" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="87">
         <v>53</v>
       </c>
       <c r="D4" s="46"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="153" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="151">
+      <c r="F4" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="90">
         <v>0</v>
       </c>
       <c r="H4" s="54"/>
       <c r="I4" s="55"/>
-      <c r="J4" s="149" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="156">
+      <c r="J4" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="95">
         <v>45</v>
       </c>
       <c r="M4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="113"/>
-      <c r="O4" s="115"/>
+      <c r="N4" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="O4" s="87">
+        <v>53</v>
+      </c>
       <c r="P4" s="46"/>
       <c r="Q4" s="6"/>
-      <c r="R4" s="108" t="s">
-        <v>43</v>
-      </c>
-      <c r="S4" s="110">
+      <c r="R4" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="90">
         <v>0</v>
       </c>
       <c r="T4" s="54"/>
       <c r="U4" s="55"/>
-      <c r="V4" s="113"/>
-      <c r="W4" s="106"/>
+      <c r="V4" s="88" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" s="95">
+        <v>45</v>
+      </c>
     </row>
     <row r="5" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="149" t="s">
+      <c r="B5" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="87">
+        <v>45</v>
+      </c>
+      <c r="D5" s="40" t="s">
         <v>36</v>
-      </c>
-      <c r="C5" s="148">
-        <v>45</v>
-      </c>
-      <c r="D5" s="40" t="s">
-        <v>38</v>
       </c>
       <c r="E5" s="41">
         <v>56</v>
       </c>
-      <c r="F5" s="153" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" s="151">
+      <c r="F5" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="90">
         <v>0</v>
       </c>
       <c r="H5" s="46"/>
       <c r="I5" s="56"/>
-      <c r="J5" s="159" t="s">
+      <c r="J5" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="157">
+      <c r="K5" s="96">
         <v>0</v>
       </c>
       <c r="M5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="N5" s="112" t="s">
+      <c r="N5" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="O5" s="87">
+        <v>45</v>
+      </c>
+      <c r="P5" s="40" t="s">
         <v>36</v>
-      </c>
-      <c r="O5" s="114">
-        <v>45</v>
-      </c>
-      <c r="P5" s="40" t="s">
-        <v>38</v>
       </c>
       <c r="Q5" s="41">
         <v>56</v>
       </c>
-      <c r="R5" s="109"/>
-      <c r="S5" s="111"/>
+      <c r="R5" s="92" t="s">
+        <v>41</v>
+      </c>
+      <c r="S5" s="90">
+        <v>0</v>
+      </c>
       <c r="T5" s="46"/>
       <c r="U5" s="56"/>
-      <c r="V5" s="127" t="s">
+      <c r="V5" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="W5" s="120">
+      <c r="W5" s="96">
         <v>0</v>
       </c>
     </row>
@@ -2918,53 +2803,61 @@
       <c r="A6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="149" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="148">
+      <c r="B6" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="87">
         <v>45</v>
       </c>
       <c r="D6" s="46"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="154" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="152">
+      <c r="F6" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="91">
         <v>73</v>
       </c>
       <c r="H6" s="43" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I6" s="44">
         <v>56</v>
       </c>
-      <c r="J6" s="159" t="s">
+      <c r="J6" s="98" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="157">
+      <c r="K6" s="96">
         <v>0</v>
       </c>
       <c r="M6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N6" s="113"/>
-      <c r="O6" s="115"/>
+      <c r="N6" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="O6" s="87">
+        <v>45</v>
+      </c>
       <c r="P6" s="46"/>
       <c r="Q6" s="6"/>
-      <c r="R6" s="116" t="s">
-        <v>44</v>
-      </c>
-      <c r="S6" s="118">
+      <c r="R6" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" s="91">
         <v>73</v>
       </c>
       <c r="T6" s="43" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U6" s="44">
         <v>56</v>
       </c>
-      <c r="V6" s="128"/>
-      <c r="W6" s="121"/>
+      <c r="V6" s="98" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="96">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -2973,43 +2866,47 @@
       <c r="B7" s="18"/>
       <c r="C7" s="8"/>
       <c r="D7" s="45" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E7" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="154" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="152">
+        <v>38</v>
+      </c>
+      <c r="F7" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="91">
         <v>73</v>
       </c>
       <c r="H7" s="45" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="I7" s="61" t="s">
-        <v>40</v>
-      </c>
-      <c r="J7" s="160"/>
-      <c r="K7" s="161"/>
+        <v>38</v>
+      </c>
+      <c r="J7" s="99"/>
+      <c r="K7" s="100"/>
       <c r="M7" s="15" t="s">
         <v>22</v>
       </c>
       <c r="N7" s="18"/>
       <c r="O7" s="8"/>
       <c r="P7" s="45" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="Q7" s="41" t="s">
-        <v>40</v>
-      </c>
-      <c r="R7" s="117"/>
-      <c r="S7" s="119"/>
+        <v>38</v>
+      </c>
+      <c r="R7" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" s="91">
+        <v>73</v>
+      </c>
       <c r="T7" s="45" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="U7" s="61" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="V7" s="18"/>
       <c r="W7" s="26"/>
@@ -3018,59 +2915,59 @@
       <c r="A8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="149" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="150">
+      <c r="B8" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="89">
         <v>33</v>
       </c>
       <c r="D8" s="47"/>
       <c r="E8" s="48"/>
-      <c r="F8" s="155" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="151">
+      <c r="F8" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="90">
         <v>0</v>
       </c>
       <c r="H8" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I8" s="62">
         <v>0</v>
       </c>
-      <c r="J8" s="149" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="158">
+      <c r="J8" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="K8" s="97">
         <v>65</v>
       </c>
       <c r="M8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="112" t="s">
-        <v>36</v>
-      </c>
-      <c r="O8" s="122">
+      <c r="N8" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="89">
         <v>33</v>
       </c>
       <c r="P8" s="47"/>
       <c r="Q8" s="48"/>
-      <c r="R8" s="124" t="s">
-        <v>41</v>
-      </c>
-      <c r="S8" s="110">
+      <c r="R8" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="S8" s="90">
         <v>0</v>
       </c>
       <c r="T8" s="29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="U8" s="62">
         <v>0</v>
       </c>
-      <c r="V8" s="112" t="s">
-        <v>44</v>
-      </c>
-      <c r="W8" s="105">
+      <c r="V8" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="W8" s="97">
         <v>65</v>
       </c>
     </row>
@@ -3078,18 +2975,18 @@
       <c r="A9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="149" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="150">
+      <c r="B9" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="89">
         <v>33</v>
       </c>
       <c r="D9" s="49"/>
       <c r="E9" s="50"/>
-      <c r="F9" s="155" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="151">
+      <c r="F9" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="90">
         <v>0</v>
       </c>
       <c r="H9" s="29" t="s">
@@ -3098,48 +2995,60 @@
       <c r="I9" s="62">
         <v>0</v>
       </c>
-      <c r="J9" s="149" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9" s="158">
+      <c r="J9" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="K9" s="97">
         <v>65</v>
       </c>
       <c r="M9" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="N9" s="113"/>
-      <c r="O9" s="123"/>
+      <c r="N9" s="88" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="89">
+        <v>33</v>
+      </c>
       <c r="P9" s="49"/>
       <c r="Q9" s="50"/>
-      <c r="R9" s="125"/>
-      <c r="S9" s="111"/>
+      <c r="R9" s="94" t="s">
+        <v>39</v>
+      </c>
+      <c r="S9" s="90">
+        <v>0</v>
+      </c>
       <c r="T9" s="29" t="s">
         <v>10</v>
       </c>
       <c r="U9" s="62">
         <v>0</v>
       </c>
-      <c r="V9" s="126"/>
-      <c r="W9" s="106"/>
+      <c r="V9" s="88" t="s">
+        <v>42</v>
+      </c>
+      <c r="W9" s="97">
+        <v>65</v>
+      </c>
     </row>
     <row r="10" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="149" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="148">
+      <c r="B10" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="87">
         <v>35</v>
       </c>
       <c r="D10" s="51"/>
       <c r="E10" s="52"/>
       <c r="F10" s="51"/>
       <c r="G10" s="52"/>
-      <c r="H10" s="155" t="s">
+      <c r="H10" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="162">
+      <c r="I10" s="101">
         <v>0</v>
       </c>
       <c r="J10" s="34"/>
@@ -3147,20 +3056,20 @@
       <c r="M10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N10" s="112" t="s">
-        <v>37</v>
-      </c>
-      <c r="O10" s="114">
+      <c r="N10" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="87">
         <v>35</v>
       </c>
       <c r="P10" s="51"/>
       <c r="Q10" s="52"/>
       <c r="R10" s="51"/>
       <c r="S10" s="52"/>
-      <c r="T10" s="124" t="s">
+      <c r="T10" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="U10" s="129">
+      <c r="U10" s="101">
         <v>0</v>
       </c>
       <c r="V10" s="34"/>
@@ -3170,20 +3079,20 @@
       <c r="A11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="149" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="148">
+      <c r="B11" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="87">
         <v>35</v>
       </c>
       <c r="D11" s="53"/>
       <c r="E11" s="50"/>
       <c r="F11" s="53"/>
       <c r="G11" s="50"/>
-      <c r="H11" s="155" t="s">
+      <c r="H11" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="162">
+      <c r="I11" s="101">
         <v>0</v>
       </c>
       <c r="J11" s="20"/>
@@ -3192,21 +3101,29 @@
       <c r="M11" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="N11" s="113"/>
-      <c r="O11" s="115"/>
+      <c r="N11" s="88" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="87">
+        <v>35</v>
+      </c>
       <c r="P11" s="53"/>
       <c r="Q11" s="50"/>
       <c r="R11" s="53"/>
       <c r="S11" s="50"/>
-      <c r="T11" s="125"/>
-      <c r="U11" s="121"/>
+      <c r="T11" s="94" t="s">
+        <v>10</v>
+      </c>
+      <c r="U11" s="101">
+        <v>0</v>
+      </c>
       <c r="V11" s="20"/>
       <c r="W11" s="32"/>
     </row>
     <row r="12" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="59" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -3216,89 +3133,67 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85"/>
-      <c r="R13" s="85"/>
-      <c r="S13" s="85"/>
-      <c r="T13" s="85"/>
-      <c r="U13" s="85"/>
-      <c r="V13" s="85"/>
+      <c r="N13" s="118"/>
+      <c r="O13" s="118"/>
+      <c r="P13" s="118"/>
+      <c r="Q13" s="118"/>
+      <c r="R13" s="118"/>
+      <c r="S13" s="118"/>
+      <c r="T13" s="118"/>
+      <c r="U13" s="118"/>
+      <c r="V13" s="118"/>
     </row>
     <row r="14" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="86"/>
-      <c r="Q14" s="86"/>
-      <c r="R14" s="86"/>
-      <c r="S14" s="86"/>
-      <c r="T14" s="86"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="86"/>
-      <c r="W14" s="86"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="108"/>
+      <c r="K14" s="108"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
+      <c r="U14" s="108"/>
+      <c r="V14" s="108"/>
+      <c r="W14" s="108"/>
     </row>
     <row r="15" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="44">
+  <mergeCells count="22">
+    <mergeCell ref="N13:V13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="O1:W1"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="M1:M2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:K1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:K2"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="O1:W1"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="V5:V6"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="N13:V13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="W8:W9"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="R4:R5"/>
-    <mergeCell ref="S4:S5"/>
-    <mergeCell ref="N5:N6"/>
-    <mergeCell ref="O5:O6"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
-    <mergeCell ref="W5:W6"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="V8:V9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3309,8 +3204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3340,113 +3235,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
-        <v>47</v>
+      <c r="A1" s="128" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="73" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="141" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="141"/>
-      <c r="E1" s="141"/>
-      <c r="F1" s="141"/>
-      <c r="G1" s="141"/>
-      <c r="H1" s="141"/>
-      <c r="I1" s="141"/>
-      <c r="J1" s="141"/>
-      <c r="K1" s="142"/>
-      <c r="M1" s="139" t="s">
-        <v>47</v>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="131"/>
+      <c r="M1" s="128" t="s">
+        <v>45</v>
       </c>
       <c r="N1" s="73" t="s">
-        <v>33</v>
-      </c>
-      <c r="O1" s="141" t="s">
+        <v>78</v>
+      </c>
+      <c r="O1" s="130" t="s">
         <v>4</v>
       </c>
-      <c r="P1" s="141"/>
-      <c r="Q1" s="141"/>
-      <c r="R1" s="141"/>
-      <c r="S1" s="141"/>
-      <c r="T1" s="141"/>
-      <c r="U1" s="141"/>
-      <c r="V1" s="141"/>
-      <c r="W1" s="142"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="130"/>
+      <c r="S1" s="130"/>
+      <c r="T1" s="130"/>
+      <c r="U1" s="130"/>
+      <c r="V1" s="130"/>
+      <c r="W1" s="131"/>
     </row>
     <row r="2" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="140"/>
+      <c r="A2" s="129"/>
       <c r="B2" s="74" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="137" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="143"/>
-      <c r="F2" s="137" t="s">
+      <c r="E2" s="132"/>
+      <c r="F2" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="143"/>
-      <c r="H2" s="144" t="s">
+      <c r="G2" s="132"/>
+      <c r="H2" s="133" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="145"/>
-      <c r="J2" s="144" t="s">
+      <c r="I2" s="134"/>
+      <c r="J2" s="133" t="s">
         <v>31</v>
       </c>
-      <c r="K2" s="145"/>
-      <c r="M2" s="140"/>
+      <c r="K2" s="134"/>
+      <c r="M2" s="129"/>
       <c r="N2" s="74" t="s">
         <v>27</v>
       </c>
       <c r="O2" s="75" t="s">
-        <v>34</v>
-      </c>
-      <c r="P2" s="137" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="126" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="143"/>
-      <c r="R2" s="137" t="s">
+      <c r="Q2" s="132"/>
+      <c r="R2" s="126" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="143"/>
-      <c r="T2" s="137" t="s">
+      <c r="S2" s="132"/>
+      <c r="T2" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="138"/>
-      <c r="V2" s="137" t="s">
+      <c r="U2" s="127"/>
+      <c r="V2" s="126" t="s">
         <v>31</v>
       </c>
-      <c r="W2" s="138"/>
+      <c r="W2" s="127"/>
     </row>
     <row r="3" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="65" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C3" s="63">
         <v>79</v>
       </c>
       <c r="D3" s="67" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E3" s="63">
         <v>143</v>
       </c>
       <c r="F3" s="67" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G3" s="63">
         <v>79</v>
       </c>
       <c r="H3" s="65" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I3" s="63">
         <v>143</v>
@@ -3457,25 +3352,25 @@
         <v>18</v>
       </c>
       <c r="N3" s="65" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="O3" s="63">
         <v>79</v>
       </c>
       <c r="P3" s="67" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="63">
         <v>143</v>
       </c>
       <c r="R3" s="67" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="S3" s="63">
         <v>79</v>
       </c>
       <c r="T3" s="65" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="U3" s="63">
         <v>143</v>
@@ -3487,14 +3382,14 @@
       <c r="A4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="146" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="147">
+      <c r="B4" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="86">
         <v>49</v>
       </c>
       <c r="D4" s="65" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E4" s="63">
         <v>112</v>
@@ -3502,13 +3397,13 @@
       <c r="F4" s="66"/>
       <c r="G4" s="64"/>
       <c r="H4" s="65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I4" s="63">
         <v>56</v>
       </c>
       <c r="J4" s="65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K4" s="63">
         <v>96</v>
@@ -3519,7 +3414,7 @@
       <c r="N4" s="69"/>
       <c r="O4" s="70"/>
       <c r="P4" s="65" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="Q4" s="63">
         <v>112</v>
@@ -3527,13 +3422,13 @@
       <c r="R4" s="66"/>
       <c r="S4" s="64"/>
       <c r="T4" s="65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="U4" s="63">
         <v>56</v>
       </c>
       <c r="V4" s="65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="W4" s="63">
         <v>96</v>
@@ -3543,32 +3438,32 @@
       <c r="A5" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="146" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="147">
+      <c r="B5" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="86">
         <v>49</v>
       </c>
       <c r="D5" s="65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E5" s="63">
         <v>107</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G5" s="63">
         <v>98</v>
       </c>
       <c r="H5" s="65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I5" s="63">
         <v>139</v>
       </c>
       <c r="J5" s="65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K5" s="63">
         <v>84</v>
@@ -3579,25 +3474,25 @@
       <c r="N5" s="68"/>
       <c r="O5" s="71"/>
       <c r="P5" s="65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="Q5" s="63">
         <v>107</v>
       </c>
       <c r="R5" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="S5" s="63">
         <v>98</v>
       </c>
       <c r="T5" s="65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="U5" s="63">
         <v>139</v>
       </c>
       <c r="V5" s="65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="W5" s="63">
         <v>84</v>
@@ -3608,25 +3503,25 @@
         <v>21</v>
       </c>
       <c r="B6" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C6" s="63">
         <v>98</v>
       </c>
       <c r="D6" s="65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" s="63">
         <v>139</v>
       </c>
       <c r="F6" s="65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G6" s="63">
         <v>74</v>
       </c>
       <c r="H6" s="65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I6" s="63">
         <v>107</v>
@@ -3637,25 +3532,25 @@
         <v>21</v>
       </c>
       <c r="N6" s="65" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="O6" s="63">
         <v>98</v>
       </c>
       <c r="P6" s="65" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="Q6" s="63">
         <v>139</v>
       </c>
       <c r="R6" s="65" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S6" s="63">
         <v>74</v>
       </c>
       <c r="T6" s="65" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="U6" s="63">
         <v>107</v>
@@ -3668,13 +3563,13 @@
         <v>22</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C7" s="72" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E7" s="63">
         <v>103</v>
@@ -3682,13 +3577,13 @@
       <c r="F7" s="66"/>
       <c r="G7" s="64"/>
       <c r="H7" s="65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="I7" s="63">
         <v>113</v>
       </c>
       <c r="J7" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K7" s="63">
         <v>103</v>
@@ -3699,7 +3594,7 @@
       <c r="N7" s="66"/>
       <c r="O7" s="64"/>
       <c r="P7" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="Q7" s="63">
         <v>103</v>
@@ -3707,13 +3602,13 @@
       <c r="R7" s="66"/>
       <c r="S7" s="64"/>
       <c r="T7" s="65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="U7" s="63">
         <v>113</v>
       </c>
       <c r="V7" s="65" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="W7" s="63">
         <v>103</v>
@@ -3724,13 +3619,13 @@
         <v>23</v>
       </c>
       <c r="B8" s="65" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="63">
         <v>66</v>
       </c>
       <c r="D8" s="65" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" s="63">
         <v>0</v>
@@ -3738,13 +3633,13 @@
       <c r="F8" s="66"/>
       <c r="G8" s="64"/>
       <c r="H8" s="65" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I8" s="63">
         <v>83</v>
       </c>
       <c r="J8" s="65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K8" s="63">
         <v>113</v>
@@ -3753,13 +3648,13 @@
         <v>23</v>
       </c>
       <c r="N8" s="65" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="O8" s="63">
         <v>66</v>
       </c>
       <c r="P8" s="65" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="Q8" s="63">
         <v>0</v>
@@ -3767,13 +3662,13 @@
       <c r="R8" s="66"/>
       <c r="S8" s="64"/>
       <c r="T8" s="65" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="U8" s="63">
         <v>83</v>
       </c>
       <c r="V8" s="65" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="W8" s="63">
         <v>113</v>
@@ -3784,19 +3679,19 @@
         <v>24</v>
       </c>
       <c r="B9" s="65" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C9" s="63">
         <v>19</v>
       </c>
       <c r="D9" s="65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E9" s="63">
         <v>108</v>
       </c>
       <c r="F9" s="65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G9" s="63">
         <v>84</v>
@@ -3813,19 +3708,19 @@
         <v>24</v>
       </c>
       <c r="N9" s="65" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="O9" s="63">
         <v>19</v>
       </c>
       <c r="P9" s="65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="Q9" s="63">
         <v>108</v>
       </c>
       <c r="R9" s="65" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S9" s="63">
         <v>84</v>
@@ -3850,7 +3745,7 @@
       <c r="F10" s="66"/>
       <c r="G10" s="64"/>
       <c r="H10" s="65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I10" s="63">
         <v>108</v>
@@ -3867,7 +3762,7 @@
       <c r="R10" s="66"/>
       <c r="S10" s="64"/>
       <c r="T10" s="65" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="U10" s="63">
         <v>108</v>
@@ -3907,7 +3802,7 @@
     <row r="12" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="59" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -3917,45 +3812,55 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85"/>
-      <c r="R13" s="85"/>
-      <c r="S13" s="85"/>
-      <c r="T13" s="85"/>
-      <c r="U13" s="85"/>
-      <c r="V13" s="85"/>
+      <c r="N13" s="118"/>
+      <c r="O13" s="118"/>
+      <c r="P13" s="118"/>
+      <c r="Q13" s="118"/>
+      <c r="R13" s="118"/>
+      <c r="S13" s="118"/>
+      <c r="T13" s="118"/>
+      <c r="U13" s="118"/>
+      <c r="V13" s="118"/>
     </row>
     <row r="14" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="60" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C14" s="58"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="N14" s="86"/>
-      <c r="O14" s="86"/>
-      <c r="P14" s="86"/>
-      <c r="Q14" s="86"/>
-      <c r="R14" s="86"/>
-      <c r="S14" s="86"/>
-      <c r="T14" s="86"/>
-      <c r="U14" s="86"/>
-      <c r="V14" s="86"/>
-      <c r="W14" s="86"/>
+      <c r="D14" s="108"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="108"/>
+      <c r="J14" s="108"/>
+      <c r="K14" s="108"/>
+      <c r="N14" s="108"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="108"/>
+      <c r="S14" s="108"/>
+      <c r="T14" s="108"/>
+      <c r="U14" s="108"/>
+      <c r="V14" s="108"/>
+      <c r="W14" s="108"/>
     </row>
     <row r="15" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:23" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="T14:U14"/>
+    <mergeCell ref="V14:W14"/>
+    <mergeCell ref="N13:V13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="P14:Q14"/>
+    <mergeCell ref="R14:S14"/>
     <mergeCell ref="T2:U2"/>
     <mergeCell ref="V2:W2"/>
     <mergeCell ref="A1:A2"/>
@@ -3968,16 +3873,6 @@
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
-    <mergeCell ref="T14:U14"/>
-    <mergeCell ref="V14:W14"/>
-    <mergeCell ref="N13:V13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="P14:Q14"/>
-    <mergeCell ref="R14:S14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -4002,25 +3897,25 @@
   <sheetData>
     <row r="1" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="76" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="76" t="s">
-        <v>76</v>
       </c>
       <c r="C1" s="76"/>
       <c r="D1" s="76"/>
       <c r="F1" s="78" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G1" s="76" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H1" s="76"/>
       <c r="I1" s="76"/>
     </row>
     <row r="2" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="81" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>0</v>
@@ -4029,10 +3924,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="83" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F2" s="82" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G2" s="15" t="s">
         <v>0</v>
@@ -4041,7 +3936,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4159,7 +4054,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="84" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="79" t="s">
         <v>22</v>
@@ -4283,7 +4178,7 @@
     </row>
     <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="81" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>0</v>
@@ -4292,10 +4187,10 @@
         <v>1</v>
       </c>
       <c r="D13" s="83" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="82" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>0</v>
@@ -4304,7 +4199,7 @@
         <v>1</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4419,7 +4314,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="77" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="83">
         <v>103</v>
@@ -4431,7 +4326,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="77" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I18" s="15">
         <v>103</v>
@@ -4546,7 +4441,7 @@
     </row>
     <row r="24" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="81" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>0</v>
@@ -4555,10 +4450,10 @@
         <v>1</v>
       </c>
       <c r="D24" s="83" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F24" s="82" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G24" s="15" t="s">
         <v>0</v>
@@ -4567,7 +4462,7 @@
         <v>1</v>
       </c>
       <c r="I24" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4809,7 +4704,7 @@
     </row>
     <row r="35" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="81" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>0</v>
@@ -4818,10 +4713,10 @@
         <v>1</v>
       </c>
       <c r="D35" s="83" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F35" s="82" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G35" s="15" t="s">
         <v>0</v>
@@ -4830,7 +4725,7 @@
         <v>1</v>
       </c>
       <c r="I35" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4945,7 +4840,7 @@
         <v>0</v>
       </c>
       <c r="C40" s="77" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D40" s="83">
         <v>113</v>
@@ -4957,7 +4852,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="77" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I40" s="15">
         <v>113</v>
@@ -5073,7 +4968,7 @@
     </row>
     <row r="46" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="81" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B46" s="15" t="s">
         <v>0</v>
@@ -5082,10 +4977,10 @@
         <v>1</v>
       </c>
       <c r="D46" s="83" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F46" s="82" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G46" s="15" t="s">
         <v>0</v>
@@ -5094,7 +4989,7 @@
         <v>1</v>
       </c>
       <c r="I46" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>